<commit_message>
Webservice, logos estados, inicializacion de datos, importacion de catalogos de excel
</commit_message>
<xml_diff>
--- a/Stock/src/main/resources/layout/LayoutProductos.xlsx
+++ b/Stock/src/main/resources/layout/LayoutProductos.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Almacen\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19710" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Inf general" sheetId="1" r:id="rId1"/>
     <sheet name="Catalogos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="222">
   <si>
     <t>nombre</t>
   </si>
@@ -868,7 +864,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -936,6 +932,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1019,7 +1021,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1038,6 +1039,7 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1056,7 +1058,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1321,10 +1323,10 @@
   <dimension ref="A1:Y30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="6"/>
     <col min="2" max="2" width="19.7109375" style="6" bestFit="1" customWidth="1"/>
@@ -1345,80 +1347,80 @@
     <col min="25" max="25" width="15" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:25" s="14" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="11" t="s">
+      <c r="E1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="S1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="T1" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="U1" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="V1" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="W1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="X1" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="Y1" s="13" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1459,10 +1461,10 @@
       <c r="L2" s="6">
         <v>34</v>
       </c>
-      <c r="M2" s="9">
-        <v>10</v>
-      </c>
-      <c r="N2" s="10">
+      <c r="M2" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N2" s="9">
         <v>2</v>
       </c>
       <c r="O2" s="6" t="s">
@@ -1536,10 +1538,10 @@
       <c r="L3" s="6">
         <v>34</v>
       </c>
-      <c r="M3" s="9">
-        <v>10</v>
-      </c>
-      <c r="N3" s="10">
+      <c r="M3" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N3" s="9">
         <v>2</v>
       </c>
       <c r="O3" s="6" t="s">
@@ -1613,10 +1615,10 @@
       <c r="L4" s="6">
         <v>34</v>
       </c>
-      <c r="M4" s="9">
-        <v>10</v>
-      </c>
-      <c r="N4" s="10">
+      <c r="M4" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N4" s="9">
         <v>2</v>
       </c>
       <c r="O4" s="6" t="s">
@@ -1690,10 +1692,10 @@
       <c r="L5" s="6">
         <v>34</v>
       </c>
-      <c r="M5" s="9">
-        <v>10</v>
-      </c>
-      <c r="N5" s="10">
+      <c r="M5" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N5" s="9">
         <v>2</v>
       </c>
       <c r="O5" s="6" t="s">
@@ -1767,10 +1769,10 @@
       <c r="L6" s="6">
         <v>34</v>
       </c>
-      <c r="M6" s="9">
-        <v>10</v>
-      </c>
-      <c r="N6" s="10">
+      <c r="M6" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N6" s="9">
         <v>2</v>
       </c>
       <c r="O6" s="6" t="s">
@@ -1844,10 +1846,10 @@
       <c r="L7" s="6">
         <v>34</v>
       </c>
-      <c r="M7" s="9">
-        <v>10</v>
-      </c>
-      <c r="N7" s="10">
+      <c r="M7" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N7" s="9">
         <v>2</v>
       </c>
       <c r="O7" s="6" t="s">
@@ -1921,10 +1923,10 @@
       <c r="L8" s="6">
         <v>34</v>
       </c>
-      <c r="M8" s="9">
-        <v>10</v>
-      </c>
-      <c r="N8" s="10">
+      <c r="M8" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N8" s="9">
         <v>2</v>
       </c>
       <c r="O8" s="6" t="s">
@@ -1998,10 +2000,10 @@
       <c r="L9" s="6">
         <v>34</v>
       </c>
-      <c r="M9" s="9">
-        <v>10</v>
-      </c>
-      <c r="N9" s="10">
+      <c r="M9" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N9" s="9">
         <v>2</v>
       </c>
       <c r="O9" s="6" t="s">
@@ -2075,10 +2077,10 @@
       <c r="L10" s="6">
         <v>34</v>
       </c>
-      <c r="M10" s="9">
-        <v>10</v>
-      </c>
-      <c r="N10" s="10">
+      <c r="M10" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N10" s="9">
         <v>2</v>
       </c>
       <c r="O10" s="6" t="s">
@@ -2152,10 +2154,10 @@
       <c r="L11" s="6">
         <v>34</v>
       </c>
-      <c r="M11" s="9">
-        <v>10</v>
-      </c>
-      <c r="N11" s="10">
+      <c r="M11" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N11" s="9">
         <v>2</v>
       </c>
       <c r="O11" s="6" t="s">
@@ -2229,10 +2231,10 @@
       <c r="L12" s="6">
         <v>34</v>
       </c>
-      <c r="M12" s="9">
-        <v>10</v>
-      </c>
-      <c r="N12" s="10">
+      <c r="M12" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N12" s="9">
         <v>2</v>
       </c>
       <c r="O12" s="6" t="s">
@@ -2306,10 +2308,10 @@
       <c r="L13" s="6">
         <v>34</v>
       </c>
-      <c r="M13" s="9">
-        <v>10</v>
-      </c>
-      <c r="N13" s="10">
+      <c r="M13" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N13" s="9">
         <v>2</v>
       </c>
       <c r="O13" s="6" t="s">
@@ -2383,10 +2385,10 @@
       <c r="L14" s="6">
         <v>34</v>
       </c>
-      <c r="M14" s="9">
-        <v>10</v>
-      </c>
-      <c r="N14" s="10">
+      <c r="M14" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N14" s="9">
         <v>2</v>
       </c>
       <c r="O14" s="6" t="s">
@@ -2460,10 +2462,10 @@
       <c r="L15" s="6">
         <v>34</v>
       </c>
-      <c r="M15" s="9">
-        <v>10</v>
-      </c>
-      <c r="N15" s="10">
+      <c r="M15" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N15" s="9">
         <v>2</v>
       </c>
       <c r="O15" s="6" t="s">
@@ -2537,10 +2539,10 @@
       <c r="L16" s="6">
         <v>34</v>
       </c>
-      <c r="M16" s="9">
-        <v>10</v>
-      </c>
-      <c r="N16" s="10">
+      <c r="M16" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N16" s="9">
         <v>2</v>
       </c>
       <c r="O16" s="6" t="s">
@@ -2614,10 +2616,10 @@
       <c r="L17" s="6">
         <v>34</v>
       </c>
-      <c r="M17" s="9">
-        <v>10</v>
-      </c>
-      <c r="N17" s="10">
+      <c r="M17" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N17" s="9">
         <v>2</v>
       </c>
       <c r="O17" s="6" t="s">
@@ -2691,10 +2693,10 @@
       <c r="L18" s="6">
         <v>34</v>
       </c>
-      <c r="M18" s="9">
-        <v>10</v>
-      </c>
-      <c r="N18" s="10">
+      <c r="M18" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N18" s="9">
         <v>2</v>
       </c>
       <c r="O18" s="6" t="s">
@@ -2768,10 +2770,10 @@
       <c r="L19" s="6">
         <v>34</v>
       </c>
-      <c r="M19" s="9">
-        <v>10</v>
-      </c>
-      <c r="N19" s="10">
+      <c r="M19" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N19" s="9">
         <v>2</v>
       </c>
       <c r="O19" s="6" t="s">
@@ -2845,10 +2847,10 @@
       <c r="L20" s="6">
         <v>34</v>
       </c>
-      <c r="M20" s="9">
-        <v>10</v>
-      </c>
-      <c r="N20" s="10">
+      <c r="M20" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N20" s="9">
         <v>2</v>
       </c>
       <c r="O20" s="6" t="s">
@@ -2922,10 +2924,10 @@
       <c r="L21" s="6">
         <v>34</v>
       </c>
-      <c r="M21" s="9">
-        <v>10</v>
-      </c>
-      <c r="N21" s="10">
+      <c r="M21" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N21" s="9">
         <v>2</v>
       </c>
       <c r="O21" s="6" t="s">
@@ -2999,10 +3001,10 @@
       <c r="L22" s="6">
         <v>34</v>
       </c>
-      <c r="M22" s="9">
-        <v>10</v>
-      </c>
-      <c r="N22" s="10">
+      <c r="M22" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N22" s="9">
         <v>2</v>
       </c>
       <c r="O22" s="6" t="s">
@@ -3076,10 +3078,10 @@
       <c r="L23" s="6">
         <v>34</v>
       </c>
-      <c r="M23" s="9">
-        <v>10</v>
-      </c>
-      <c r="N23" s="10">
+      <c r="M23" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N23" s="9">
         <v>2</v>
       </c>
       <c r="O23" s="6" t="s">
@@ -3153,10 +3155,10 @@
       <c r="L24" s="6">
         <v>34</v>
       </c>
-      <c r="M24" s="9">
-        <v>10</v>
-      </c>
-      <c r="N24" s="10">
+      <c r="M24" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N24" s="9">
         <v>2</v>
       </c>
       <c r="O24" s="6" t="s">
@@ -3230,10 +3232,10 @@
       <c r="L25" s="6">
         <v>34</v>
       </c>
-      <c r="M25" s="9">
-        <v>10</v>
-      </c>
-      <c r="N25" s="10">
+      <c r="M25" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N25" s="9">
         <v>2</v>
       </c>
       <c r="O25" s="6" t="s">
@@ -3307,10 +3309,10 @@
       <c r="L26" s="6">
         <v>34</v>
       </c>
-      <c r="M26" s="9">
-        <v>10</v>
-      </c>
-      <c r="N26" s="10">
+      <c r="M26" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N26" s="9">
         <v>2</v>
       </c>
       <c r="O26" s="6" t="s">
@@ -3384,10 +3386,10 @@
       <c r="L27" s="6">
         <v>34</v>
       </c>
-      <c r="M27" s="9">
-        <v>10</v>
-      </c>
-      <c r="N27" s="10">
+      <c r="M27" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N27" s="9">
         <v>2</v>
       </c>
       <c r="O27" s="6" t="s">
@@ -3461,10 +3463,10 @@
       <c r="L28" s="6">
         <v>34</v>
       </c>
-      <c r="M28" s="9">
-        <v>10</v>
-      </c>
-      <c r="N28" s="10">
+      <c r="M28" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N28" s="9">
         <v>2</v>
       </c>
       <c r="O28" s="6" t="s">
@@ -3538,10 +3540,10 @@
       <c r="L29" s="6">
         <v>34</v>
       </c>
-      <c r="M29" s="9">
-        <v>10</v>
-      </c>
-      <c r="N29" s="10">
+      <c r="M29" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N29" s="9">
         <v>2</v>
       </c>
       <c r="O29" s="6" t="s">
@@ -3615,10 +3617,10 @@
       <c r="L30" s="6">
         <v>34</v>
       </c>
-      <c r="M30" s="9">
-        <v>10</v>
-      </c>
-      <c r="N30" s="10">
+      <c r="M30" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="N30" s="9">
         <v>2</v>
       </c>
       <c r="O30" s="6" t="s">
@@ -3669,26 +3671,26 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="18" t="s">
+      <c r="D1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="18"/>
+      <c r="F1" s="17"/>
       <c r="G1" s="5"/>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="19"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>